<commit_message>
Changes in file name
</commit_message>
<xml_diff>
--- a/Wyniki.xlsx
+++ b/Wyniki.xlsx
@@ -442,28 +442,28 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <v>0.8888888888888888</v>
+        <v>0.8925</v>
       </c>
       <c r="C2">
-        <v>0.975</v>
+        <v>0.0025</v>
       </c>
       <c r="D2">
-        <v>0.9135802469135802</v>
+        <v>0.865</v>
       </c>
       <c r="E2">
-        <v>0.8375</v>
+        <v>0.9</v>
       </c>
       <c r="F2">
-        <v>0.8625</v>
+        <v>0.8825</v>
       </c>
       <c r="G2">
-        <v>0.8</v>
+        <v>0.8875</v>
       </c>
       <c r="H2">
-        <v>0.875</v>
+        <v>0.855</v>
       </c>
       <c r="I2">
-        <v>0.857716049382716</v>
+        <v>0.8780000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -471,28 +471,28 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>0.9135802469135802</v>
+        <v>0.8475</v>
       </c>
       <c r="C3">
-        <v>0.905</v>
+        <v>0.005</v>
       </c>
       <c r="D3">
-        <v>0.9135802469135802</v>
+        <v>0.835</v>
       </c>
       <c r="E3">
-        <v>0.85</v>
+        <v>0.855</v>
       </c>
       <c r="F3">
+        <v>0.8375</v>
+      </c>
+      <c r="G3">
         <v>0.8625</v>
       </c>
-      <c r="G3">
-        <v>0.7875</v>
-      </c>
       <c r="H3">
-        <v>0.9</v>
+        <v>0.84</v>
       </c>
       <c r="I3">
-        <v>0.8627160493827161</v>
+        <v>0.8459999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -500,28 +500,28 @@
         <v>11</v>
       </c>
       <c r="B4">
-        <v>0.8765432098765432</v>
+        <v>0.825</v>
       </c>
       <c r="C4">
-        <v>0.8774999999999999</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>0.8888888888888888</v>
+        <v>0.835</v>
       </c>
       <c r="E4">
-        <v>0.85</v>
+        <v>0.825</v>
       </c>
       <c r="F4">
-        <v>0.85</v>
+        <v>0.8275</v>
       </c>
       <c r="G4">
-        <v>0.7875</v>
+        <v>0.83</v>
       </c>
       <c r="H4">
-        <v>0.9</v>
+        <v>0.79</v>
       </c>
       <c r="I4">
-        <v>0.8552777777777779</v>
+        <v>0.8215</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -529,28 +529,28 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <v>0.8271604938271605</v>
+        <v>0.8275</v>
       </c>
       <c r="C5">
-        <v>0.9625</v>
+        <v>0.0175</v>
       </c>
       <c r="D5">
-        <v>0.8395061728395061</v>
+        <v>0.79</v>
       </c>
       <c r="E5">
-        <v>0.8</v>
+        <v>0.8125</v>
       </c>
       <c r="F5">
-        <v>0.85</v>
+        <v>0.8075</v>
       </c>
       <c r="G5">
-        <v>0.775</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="H5">
-        <v>0.8375</v>
+        <v>0.77</v>
       </c>
       <c r="I5">
-        <v>0.8204012345679013</v>
+        <v>0.798</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -558,28 +558,28 @@
         <v>13</v>
       </c>
       <c r="B6">
-        <v>0.8518518518518519</v>
+        <v>0.82</v>
       </c>
       <c r="C6">
-        <v>0.885</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>0.8765432098765432</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="E6">
-        <v>0.8375</v>
+        <v>0.7975</v>
       </c>
       <c r="F6">
-        <v>0.85</v>
+        <v>0.835</v>
       </c>
       <c r="G6">
-        <v>0.7875</v>
+        <v>0.8325</v>
       </c>
       <c r="H6">
-        <v>0.9125</v>
+        <v>0.8</v>
       </c>
       <c r="I6">
-        <v>0.8528086419753086</v>
+        <v>0.8160000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -587,28 +587,28 @@
         <v>14</v>
       </c>
       <c r="B7">
-        <v>0.7407407407407407</v>
+        <v>0.65</v>
       </c>
       <c r="C7">
-        <v>0.775</v>
+        <v>0.005</v>
       </c>
       <c r="D7">
-        <v>0.5679012345679012</v>
+        <v>0.5649999999999999</v>
       </c>
       <c r="E7">
-        <v>0.575</v>
+        <v>0.535</v>
       </c>
       <c r="F7">
-        <v>0.65</v>
+        <v>0.535</v>
       </c>
       <c r="G7">
-        <v>0.6875</v>
+        <v>0.5375</v>
       </c>
       <c r="H7">
-        <v>0.75</v>
+        <v>0.515</v>
       </c>
       <c r="I7">
-        <v>0.6460802469135802</v>
+        <v>0.5375000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -616,28 +616,28 @@
         <v>15</v>
       </c>
       <c r="B8">
-        <v>0.8641975308641975</v>
+        <v>0.9175</v>
       </c>
       <c r="C8">
-        <v>0.9025</v>
+        <v>0.0025</v>
       </c>
       <c r="D8">
-        <v>0.8641975308641975</v>
+        <v>0.885</v>
       </c>
       <c r="E8">
-        <v>0.8125</v>
+        <v>0.89</v>
       </c>
       <c r="F8">
-        <v>0.85</v>
+        <v>0.89</v>
       </c>
       <c r="G8">
-        <v>0.775</v>
+        <v>0.8825</v>
       </c>
       <c r="H8">
-        <v>0.9</v>
+        <v>0.8575</v>
       </c>
       <c r="I8">
-        <v>0.8403395061728395</v>
+        <v>0.881</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -645,28 +645,28 @@
         <v>16</v>
       </c>
       <c r="B9">
-        <v>0.8888888888888888</v>
+        <v>0.9275</v>
       </c>
       <c r="C9">
-        <v>0.9725</v>
+        <v>0.01</v>
       </c>
       <c r="D9">
-        <v>0.9135802469135802</v>
+        <v>0.89</v>
       </c>
       <c r="E9">
+        <v>0.9075</v>
+      </c>
+      <c r="F9">
+        <v>0.905</v>
+      </c>
+      <c r="G9">
+        <v>0.895</v>
+      </c>
+      <c r="H9">
         <v>0.875</v>
       </c>
-      <c r="F9">
-        <v>0.875</v>
-      </c>
-      <c r="G9">
-        <v>0.8</v>
-      </c>
-      <c r="H9">
-        <v>0.9125</v>
-      </c>
       <c r="I9">
-        <v>0.875216049382716</v>
+        <v>0.8945000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -674,28 +674,28 @@
         <v>17</v>
       </c>
       <c r="B10">
-        <v>0.8641975308641975</v>
+        <v>0.8925</v>
       </c>
       <c r="C10">
-        <v>0.9725</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>0.8765432098765432</v>
+        <v>0.8725000000000001</v>
       </c>
       <c r="E10">
-        <v>0.8125</v>
+        <v>0.87</v>
       </c>
       <c r="F10">
-        <v>0.8375</v>
+        <v>0.88</v>
       </c>
       <c r="G10">
-        <v>0.75</v>
+        <v>0.885</v>
       </c>
       <c r="H10">
-        <v>0.8375</v>
+        <v>0.85</v>
       </c>
       <c r="I10">
-        <v>0.8228086419753087</v>
+        <v>0.8714999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -703,28 +703,28 @@
         <v>18</v>
       </c>
       <c r="B11">
-        <v>0.8888888888888888</v>
+        <v>0.9275</v>
       </c>
       <c r="C11">
-        <v>0.945</v>
+        <v>0.01</v>
       </c>
       <c r="D11">
-        <v>0.9135802469135802</v>
+        <v>0.895</v>
       </c>
       <c r="E11">
-        <v>0.85</v>
+        <v>0.905</v>
       </c>
       <c r="F11">
-        <v>0.8625</v>
+        <v>0.905</v>
       </c>
       <c r="G11">
-        <v>0.8</v>
+        <v>0.8975</v>
       </c>
       <c r="H11">
-        <v>0.9125</v>
+        <v>0.88</v>
       </c>
       <c r="I11">
-        <v>0.867716049382716</v>
+        <v>0.8965</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Files updated (number of classes have to be equal).
</commit_message>
<xml_diff>
--- a/Wyniki.xlsx
+++ b/Wyniki.xlsx
@@ -445,25 +445,25 @@
         <v>0.9125</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>0.845</v>
       </c>
       <c r="D2">
-        <v>0.875</v>
+        <v>0.8625</v>
       </c>
       <c r="E2">
-        <v>0.8925</v>
+        <v>0.89</v>
       </c>
       <c r="F2">
-        <v>0.875</v>
+        <v>0.8825</v>
       </c>
       <c r="G2">
-        <v>0.885</v>
+        <v>0.88</v>
       </c>
       <c r="H2">
-        <v>0.8475</v>
+        <v>0.855</v>
       </c>
       <c r="I2">
-        <v>0.875</v>
+        <v>0.8739999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -474,7 +474,7 @@
         <v>0.8475</v>
       </c>
       <c r="C3">
-        <v>0.005</v>
+        <v>0.78</v>
       </c>
       <c r="D3">
         <v>0.835</v>
@@ -503,7 +503,7 @@
         <v>0.825</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.745</v>
       </c>
       <c r="D4">
         <v>0.835</v>
@@ -529,28 +529,28 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <v>0.835</v>
+        <v>0.845</v>
       </c>
       <c r="C5">
-        <v>0.0225</v>
+        <v>0.7524999999999999</v>
       </c>
       <c r="D5">
-        <v>0.8025</v>
+        <v>0.8</v>
       </c>
       <c r="E5">
-        <v>0.8175</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="F5">
-        <v>0.8149999999999999</v>
+        <v>0.8</v>
       </c>
       <c r="G5">
-        <v>0.8125</v>
+        <v>0.8275</v>
       </c>
       <c r="H5">
-        <v>0.78</v>
+        <v>0.7675</v>
       </c>
       <c r="I5">
-        <v>0.8055</v>
+        <v>0.8019999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -561,7 +561,7 @@
         <v>0.82</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>0.6925</v>
       </c>
       <c r="D6">
         <v>0.8149999999999999</v>
@@ -590,7 +590,7 @@
         <v>0.65</v>
       </c>
       <c r="C7">
-        <v>0.005</v>
+        <v>0.4075</v>
       </c>
       <c r="D7">
         <v>0.5649999999999999</v>
@@ -619,7 +619,7 @@
         <v>0.9175</v>
       </c>
       <c r="C8">
-        <v>0.0025</v>
+        <v>0.8325</v>
       </c>
       <c r="D8">
         <v>0.885</v>
@@ -648,7 +648,7 @@
         <v>0.9275</v>
       </c>
       <c r="C9">
-        <v>0.01</v>
+        <v>0.86</v>
       </c>
       <c r="D9">
         <v>0.89</v>
@@ -677,7 +677,7 @@
         <v>0.8925</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>0.82</v>
       </c>
       <c r="D10">
         <v>0.8725000000000001</v>
@@ -706,7 +706,7 @@
         <v>0.9275</v>
       </c>
       <c r="C11">
-        <v>0.01</v>
+        <v>0.8575</v>
       </c>
       <c r="D11">
         <v>0.895</v>

</xml_diff>